<commit_message>
Updating BB pathway. Currently an issue with importing to BB_Spine_DB
</commit_message>
<xml_diff>
--- a/.spinetoolbox/items/toward_bb/output/exported.xlsx
+++ b/.spinetoolbox/items/toward_bb/output/exported.xlsx
@@ -7,11 +7,13 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="node" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="demand" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="p_unit" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="node__commodity" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="node__unit__io" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="demand" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="p_unit" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="node__unit__io" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="node" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="unit" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="commodity" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="p_commodity_price" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -349,40 +351,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nodeElec</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>nodeGas</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,52 +367,59 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2020-01-01T00:00:00</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>80</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-01T01:00:00</t>
+          <t>2020-01-01T00:00:00</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-01-01T02:00:00</t>
+          <t>2020-01-01T01:00:00</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-01-01T03:00:00</t>
+          <t>2020-01-01T02:00:00</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2020-01-01T03:00:00</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>2020-01-01T04:00:00</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>73</v>
       </c>
     </row>
@@ -452,13 +428,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,17 +445,22 @@
     <row r="1">
       <c r="C1" t="inlineStr">
         <is>
-          <t>efficiency_full_load</t>
+          <t>eff00</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>efficiency_min_load</t>
+          <t>eff01</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>min_load</t>
+          <t>op00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>op01</t>
         </is>
       </c>
     </row>
@@ -495,14 +476,17 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.4</v>
       </c>
       <c r="E2" t="n">
         <v>0.3</v>
       </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -515,7 +499,7 @@
           <t>High</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -524,38 +508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nodeGas</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>gas</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -589,4 +542,190 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>gas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>nodeElec</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>gas</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>gas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2020-01-01T00:00:00</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2020-01-01T01:00:00</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2020-01-01T02:00:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2020-01-01T03:00:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2020-01-01T04:00:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Better workflow for Backbone. Not full yet.
</commit_message>
<xml_diff>
--- a/.spinetoolbox/items/toward_bb/output/exported.xlsx
+++ b/.spinetoolbox/items/toward_bb/output/exported.xlsx
@@ -376,7 +376,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-01T00:00:00</t>
+          <t>t000001</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -386,7 +386,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-01-01T01:00:00</t>
+          <t>t000002</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -396,7 +396,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-01-01T02:00:00</t>
+          <t>t000003</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -406,7 +406,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-01-01T03:00:00</t>
+          <t>t000004</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -416,7 +416,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-01-01T04:00:00</t>
+          <t>t000005</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,23 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>output</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>gas</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
     </row>
@@ -635,7 +652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,7 +670,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-01-01T00:00:00</t>
+          <t>t000001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -662,66 +679,6 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2020-01-01T01:00:00</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2020-01-01T02:00:00</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2020-01-01T03:00:00</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2020-01-01T04:00:00</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to the BB database and exporter to BB
</commit_message>
<xml_diff>
--- a/.spinetoolbox/items/toward_bb/output/exported.xlsx
+++ b/.spinetoolbox/items/toward_bb/output/exported.xlsx
@@ -13,10 +13,10 @@
     <sheet name="unit" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="commodity" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="p_commodity_price" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="capacityFactor" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="reserveDemand" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="unit_ts" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="p_unit" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reserveDemand" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="unit_ts" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="unit_p" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="flow" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,78 +446,110 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>wind1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gas_turbine</t>
+          <t>capacityFactor</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eff00</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>t000001</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gas_turbine</t>
+          <t>capacityFactor</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eff01</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.5</v>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>t000002</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gas_turbine</t>
+          <t>capacityFactor</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>op00</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.3</v>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>t000003</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>gas_turbine</t>
+          <t>capacityFactor</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>op01</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>t000004</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>capacityFactor</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>t000005</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -724,150 +756,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>wind1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>capacityFactor</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>t000001</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>wind1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>capacityFactor</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>t000002</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>wind1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>capacityFactor</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>t000003</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>wind1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>capacityFactor</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>t000004</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>wind1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>capacityFactor</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>t000005</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -917,13 +805,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,28 +820,124 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>gas_turbine</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Base</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>eff01_ts</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>t000001</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
       <c r="C1" t="inlineStr">
         <is>
-          <t>eff01_ts</t>
+          <t>Base</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>t000001</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>eff00</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>eff01</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>0.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>op00</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>gas_turbine</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>op01</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>